<commit_message>
First commit to this branch
</commit_message>
<xml_diff>
--- a/table_data_teams.xlsx
+++ b/table_data_teams.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,12 +465,12 @@
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Sarb</t>
+          <t>Sandeep</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Ajay</t>
+          <t>--</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -479,12 +479,12 @@
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Danish</t>
+          <t>Ajay</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>RamanSShakilAAjay+ 1RKRaman KSKShakil KAKAjay KRKRamandeep Kaur</t>
+          <t>1Member 1M4Member 4MFMEmber five+ 1M1Member 1 C by OwnerM4Member 4 C by admin 1MFMEmber five created by Admin oneTTtest test</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
@@ -493,15 +493,29 @@
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Hitesh</t>
+          <t>Team 1 created by Admin 1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>AjayRRamandeep</t>
+          <t>4Member 4MFMEmber five</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Team 3 edited by owner 2</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>3Admin 3M4Member 4MFMEmber five</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>